<commit_message>
Fixing sending bulk emails error in reading excel sheet
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Certifier\github\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E681DB-B756-4CD0-AFAE-57F551637DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFC7649-F002-4FAE-B9A0-02A7EC464B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9F5027E3-67D1-4F3A-8710-4CE03C6CABA5}"/>
+    <workbookView xWindow="5190" yWindow="1470" windowWidth="28800" windowHeight="15435" xr2:uid="{9F5027E3-67D1-4F3A-8710-4CE03C6CABA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="A2:C4"/>
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>